<commit_message>
add apache poi reader
</commit_message>
<xml_diff>
--- a/src/main/resources/Example.xlsx
+++ b/src/main/resources/Example.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\Projetos\Fullstack\Readfile\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920D6E04-EED0-4069-B793-9C3399460619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814A908-A4C6-4ACF-9FE7-60FCD762A019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2A87FE54-3E15-4E5A-8348-34F14E0DC3D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Teste" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>titulo</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>clean code</t>
   </si>
@@ -415,34 +406,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8166741A-0BCC-4545-843B-6F33320F94A1}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,10 +427,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validate header and body row
</commit_message>
<xml_diff>
--- a/src/main/resources/Example.xlsx
+++ b/src/main/resources/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\Projetos\Fullstack\Readfile\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814A908-A4C6-4ACF-9FE7-60FCD762A019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E088A9AA-772D-41D0-BBD0-1A81F34C1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2A87FE54-3E15-4E5A-8348-34F14E0DC3D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>clean code</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Victor</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>titulo</t>
   </si>
 </sst>
 </file>
@@ -406,15 +415,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8166741A-0BCC-4545-843B-6F33320F94A1}">
-  <dimension ref="A2:C3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>

</xml_diff>